<commit_message>
Dodanie plików oraz aktualizacja
</commit_message>
<xml_diff>
--- a/Przypadki testowe - Api Trello.xlsx
+++ b/Przypadki testowe - Api Trello.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sylwia\OneDrive - Office 365\Pulpit\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repozytorium\Postman-Api-Trello\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="60">
   <si>
     <t>Nazwa testu</t>
   </si>
@@ -55,17 +55,67 @@
   </si>
   <si>
     <t>1. Kliknij przycisk "Utwórz" znajdujący się w panelu na górze ekranu</t>
-  </si>
-  <si>
-    <t>Utworzenie nowej nowej listy</t>
-  </si>
-  <si>
-    <t>Celem testu jest utworzenie listy w tablicy.</t>
   </si>
   <si>
     <t>1. Użytkownik powinien posiadać konto na www.trello.com 
 2. Otwarta w przeglądarce strona www.trello.com
 3. Użytkownik powinien mieć utworzoną tablicę</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>P001</t>
+  </si>
+  <si>
+    <t>Spodziewany rezultat</t>
+  </si>
+  <si>
+    <t>Autor</t>
+  </si>
+  <si>
+    <t>Sylwia Sakwa</t>
+  </si>
+  <si>
+    <t>P002</t>
+  </si>
+  <si>
+    <t>P003</t>
+  </si>
+  <si>
+    <t>P004</t>
+  </si>
+  <si>
+    <t>P005</t>
+  </si>
+  <si>
+    <t>Utworzenie nowej etykiety</t>
+  </si>
+  <si>
+    <t>Celem testu jest utworzenie nowej etykiety</t>
+  </si>
+  <si>
+    <t>Aktualizacja nazwy tablicy</t>
+  </si>
+  <si>
+    <t>Celem testu jest zaktualizowanie nazwy tablicy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Użytkownik powinien posiadać konto na www.trello.com 
+2. Otwarta w przeglądarce strona www.trello.com
+3. Użytkownik powinien mieć utworzoną tablicę </t>
+  </si>
+  <si>
+    <t>1. Wejdź w tablicę
+2. Kliknij w nazwę tablicy
+3. Zmień nazwę 
+4. Naciśnij "enter"</t>
+  </si>
+  <si>
+    <t>Nazwa tablicy jest taka jaką nadał użytkownik przy edycji</t>
+  </si>
+  <si>
+    <t>Celem testu jest utworzenie listy w tablicy.</t>
   </si>
   <si>
     <t>1. Wejdź w tablicę
@@ -77,33 +127,142 @@
     <t>Na tablicy pojawia się nowa lista</t>
   </si>
   <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>P001</t>
-  </si>
-  <si>
-    <t>Spodziewany rezultat</t>
-  </si>
-  <si>
-    <t>Dane testowe</t>
-  </si>
-  <si>
-    <t>Autor</t>
-  </si>
-  <si>
-    <t>Sylwia Sakwa</t>
-  </si>
-  <si>
-    <t>P002</t>
+    <t>Celem testu jest zaltualizowanie nazwy listy</t>
+  </si>
+  <si>
+    <t>Aktualizacja nazwy listy na tablicy</t>
+  </si>
+  <si>
+    <t>Utworzenie nowej listy na tablicy</t>
+  </si>
+  <si>
+    <t>1. Użytkownik powinien posiadać konto na www.trello.com 
+2. Otwarta w przeglądarce strona www.trello.com
+3. Użytkownik powinien mieć utworzoną tablicę
+4. Użytkownik powinien mieć utworzoną listę na tablicy</t>
+  </si>
+  <si>
+    <t>1. Wejdź w tablicę
+2. Kliknij w nazwę listy
+3. Zmień nazwę
+4. Kliknij "enter"</t>
+  </si>
+  <si>
+    <t>Nazwa listy jest taka jaką nadał użytkownik przy edycji</t>
+  </si>
+  <si>
+    <t>Nazwa tablicy zaktualizowała się</t>
+  </si>
+  <si>
+    <t>Nazwa listy zaktualizowała się</t>
+  </si>
+  <si>
+    <t>Dodanie nowej karty do listy</t>
+  </si>
+  <si>
+    <t>Celem testu jest dodanie nowej karty do listy</t>
+  </si>
+  <si>
+    <t>1. Wejdź w tablicę
+2. Kliknij przycisk "dodaj kartę"
+3. Wprowadź tytuł dla tej karty
+4. Kliknij przycisk "Dodaj kartę"</t>
+  </si>
+  <si>
+    <t>Karta została dodana do listy</t>
+  </si>
+  <si>
+    <t>P006</t>
+  </si>
+  <si>
+    <t>P007</t>
+  </si>
+  <si>
+    <t>1. Użytkownik powinien posiadać konto na www.trello.com 
+2. Otwarta w przeglądarce strona www.trello.com
+3. Użytkownik powinien mieć utworzoną tablicę
+4. Użytkownik powinien mieć utworzoną listę na tablicy wraz z kartą</t>
+  </si>
+  <si>
+    <t>1. Wejdź w tablicę
+2. Kliknij w kartę na liście
+3. Kliknij w przycisk "Etykiety"
+4. Kliknij "Utwórz nową etykietę"
+5. Wprowadź tytuł etykiety
+6. Wybierz kolor
+7. Kliknij "Utwórz"</t>
+  </si>
+  <si>
+    <t>Etykieta o wybranym kolorze i nazwie została dodana</t>
+  </si>
+  <si>
+    <t>Nowa etykieta pojawiła się w proponowanych etykietach</t>
+  </si>
+  <si>
+    <t>P008</t>
+  </si>
+  <si>
+    <t>Usunięcie karty</t>
+  </si>
+  <si>
+    <t>Usunięcie tablicy</t>
+  </si>
+  <si>
+    <t>Celem testu jest usunięcie karty</t>
+  </si>
+  <si>
+    <t>1. Użytkownik powinien posiadać konto na www.trello.com 
+2. Otwarta w przeglądarce strona www.trello.com
+3. Użytkownik powinien mieć utworzoną tablicę
+4. Użytkownik powinien mieć utworzoną listę na tablicy oraz kartę</t>
+  </si>
+  <si>
+    <t>Karta została usunięta z listy</t>
+  </si>
+  <si>
+    <t>Karty nie ma na liście.</t>
+  </si>
+  <si>
+    <t>1. Wejdź na tablicę
+2. Kliknij na kartę
+3. Kliknij przycisk "Zarchiwizuj"
+4. Kliknij przycisk "Usuń"
+5. Kliknij przycisk "Skasuj"</t>
+  </si>
+  <si>
+    <t>Celem testu jest usunięcie tablicy</t>
+  </si>
+  <si>
+    <t>1. Wejdź na tablicę
+2. Kliknij w trzy kropki po prawej stronie ekranu
+3. Kliknij "Więcej"
+4. Kliknij "Zamknij tablicę"
+5. Kliknij "Zamknij"
+6. Kliknij "Trwale usuń tablicę"
+7. Kliknij "Usuń"</t>
+  </si>
+  <si>
+    <t>W oknie informacyjnym jest informacja, że trwa usuwanie tablicy.</t>
+  </si>
+  <si>
+    <t>Tablica zniknęła z przestrzeni roboczej</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -170,10 +329,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -456,10 +615,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="A69" sqref="A69:B76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -475,15 +634,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>16</v>
+      <c r="A1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -491,7 +650,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -499,7 +658,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -507,7 +666,7 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -515,15 +674,15 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
-        <v>17</v>
+      <c r="A6" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -531,87 +690,459 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="2"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>20</v>
+      <c r="A8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A15" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19" s="2"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A33" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A34" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B39" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="2" t="s">
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B40" s="2" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="A42" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A43" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A52" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A53" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A59" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A62" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="A63" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A64" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A65" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A66" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A69" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B69" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A70" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A71" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A72" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A73" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A74" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A75" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A76" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>